<commit_message>
add res boundary attack for SEED 77
</commit_message>
<xml_diff>
--- a/results/SEED_77/result.xlsx
+++ b/results/SEED_77/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>30.68317413330078</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>3.365715980529785</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>3.425267219543457</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>3.436357021331787</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>3.506391763687134</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>3.66422963142395</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>3.871299743652344</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>4.294879913330078</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>6.093916416168213</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>31.10054299227045</v>
       </c>
+      <c r="AS5" t="n">
+        <v>4.391582561076026</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>4.453119003559559</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>4.482705898885552</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>4.57630504067609</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>4.677706647882333</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>5.035980654302863</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>5.408472387155367</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>7.571858566083719</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9841685891151428</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9996684193611145</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.9996588230133057</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9996528029441833</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9996389746665955</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9996217489242554</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9995622634887695</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9994813203811646</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.998970627784729</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>40.15118408203125</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3.456785678863525</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>3.548597812652588</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.804541110992432</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>4.195152759552002</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>4.487371444702148</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>5.448037624359131</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>6.861483573913574</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>11.56615543365479</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>40.33565831905127</v>
       </c>
+      <c r="AS8" t="n">
+        <v>4.342254381189789</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>4.439331321539029</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>4.785290176697262</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>5.277365435281131</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>5.639112444091223</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>6.805521619370461</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>8.545227003480694</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>14.57730227782969</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.9771521687507629</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997920989990234</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997710585594177</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.999718189239502</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996262788772583</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9995540976524353</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9992905259132385</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9988683462142944</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9963282942771912</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>30.04141426086426</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>3.063418388366699</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>3.161049604415894</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.251139879226685</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.56424355506897</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.829797983169556</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.520462512969971</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.508560180664062</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>8.935407638549805</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>30.26114770703311</v>
       </c>
+      <c r="AS11" t="n">
+        <v>3.99095669341003</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4.066556343291467</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>4.205771368265758</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.511735871517837</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>4.897603379191018</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>5.702020240279461</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>6.943561002698353</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>11.18518656248075</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9849032759666443</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997690916061401</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997552037239075</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997372627258301</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996918439865112</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996218681335449</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9994951486587524</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.999189555644989</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9978799819946289</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>